<commit_message>
check also for currency
</commit_message>
<xml_diff>
--- a/src/grades.xlsx
+++ b/src/grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iremd\OneDrive\Masaüstü\frontend_cs401\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD349AF5-D3B7-48DF-A2D9-BA1000D93415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4475003D-0449-453B-A0A9-34C91C73CA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -176,9 +176,6 @@
     <t>Virtualtour</t>
   </si>
   <si>
-    <t>Weatherforecast</t>
-  </si>
-  <si>
     <t>Bookbutton</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>عربي</t>
+  </si>
+  <si>
+    <t>Weather</t>
   </si>
 </sst>
 </file>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,7 +750,7 @@
     </row>
     <row r="13" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="14">
         <v>2.4875621890547261</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="16" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="6">
         <v>0.49751243781094523</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="18" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="7">
         <v>2.4875621890547261</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="19" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="7">
         <v>2.4875621890547261</v>
@@ -806,7 +806,7 @@
     </row>
     <row r="20" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="7">
         <v>2.4875621890547301</v>
@@ -814,7 +814,7 @@
     </row>
     <row r="21" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="7">
         <v>1.9900497512437809</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="22" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="7">
         <v>1.4925373134328357</v>
@@ -830,7 +830,7 @@
     </row>
     <row r="23" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="7">
         <v>1.4925373134328399</v>
@@ -838,7 +838,7 @@
     </row>
     <row r="24" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="7">
         <v>1.4925373134328399</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="31" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B31" s="7">
         <v>1.9900497512437809</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="41" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B41" s="7">
         <v>2.4875621890547261</v>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="59" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B59" s="7">
         <v>1.9900497512437809</v>

</xml_diff>

<commit_message>
final version before presentaion
</commit_message>
<xml_diff>
--- a/src/grades.xlsx
+++ b/src/grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iremd\OneDrive\Masaüstü\frontend_cs401\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4475003D-0449-453B-A0A9-34C91C73CA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A6C781-A408-409F-9943-1863C349965B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="948" yWindow="2544" windowWidth="17304" windowHeight="8892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,124 +92,124 @@
     <t>About</t>
   </si>
   <si>
+    <t>Photo</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Amenities</t>
+  </si>
+  <si>
+    <t>Reservation</t>
+  </si>
+  <si>
+    <t>Arrival</t>
+  </si>
+  <si>
+    <t>Departure</t>
+  </si>
+  <si>
+    <t>Gallery</t>
+  </si>
+  <si>
+    <t>Subscription</t>
+  </si>
+  <si>
+    <t>User Interface</t>
+  </si>
+  <si>
+    <t>Slider</t>
+  </si>
+  <si>
+    <t>Hotel Policies</t>
+  </si>
+  <si>
+    <t>User Experience</t>
+  </si>
+  <si>
+    <t>Chatbot</t>
+  </si>
+  <si>
+    <t>QuestionForm</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>Certificate</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Searchbar</t>
+  </si>
+  <si>
+    <t>Journal</t>
+  </si>
+  <si>
+    <t>Newsletter</t>
+  </si>
+  <si>
+    <t>Virtualtour</t>
+  </si>
+  <si>
+    <t>Bookbutton</t>
+  </si>
+  <si>
+    <t>Aboutus</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>Türkçe</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Русский</t>
+  </si>
+  <si>
+    <t>Deutsch</t>
+  </si>
+  <si>
+    <t>Español</t>
+  </si>
+  <si>
+    <t>Italiano</t>
+  </si>
+  <si>
+    <t>عربي</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>Survey</t>
+  </si>
+  <si>
+    <t>Cancellation</t>
+  </si>
+  <si>
+    <t>Cookie_policy</t>
+  </si>
+  <si>
+    <t>Privacy_policy</t>
+  </si>
+  <si>
+    <t>Special_offer</t>
+  </si>
+  <si>
+    <t>Policies</t>
+  </si>
+  <si>
     <t>Location</t>
-  </si>
-  <si>
-    <t>Photo</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Amenities</t>
-  </si>
-  <si>
-    <t>Reservation</t>
-  </si>
-  <si>
-    <t>Arrival</t>
-  </si>
-  <si>
-    <t>Departure</t>
-  </si>
-  <si>
-    <t>Gallery</t>
-  </si>
-  <si>
-    <t>Subscription</t>
-  </si>
-  <si>
-    <t>User Interface</t>
-  </si>
-  <si>
-    <t>Slider</t>
-  </si>
-  <si>
-    <t>Hotel Policies</t>
-  </si>
-  <si>
-    <t>User Experience</t>
-  </si>
-  <si>
-    <t>Chatbot</t>
-  </si>
-  <si>
-    <t>QuestionForm</t>
-  </si>
-  <si>
-    <t>Adult</t>
-  </si>
-  <si>
-    <t>Certificate</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>Form</t>
-  </si>
-  <si>
-    <t>Cookiepolicy</t>
-  </si>
-  <si>
-    <t>Cancellationpolicy</t>
-  </si>
-  <si>
-    <t>Privacypolicy</t>
-  </si>
-  <si>
-    <t>Hotelpolicy</t>
-  </si>
-  <si>
-    <t>Searchbar</t>
-  </si>
-  <si>
-    <t>Specialoffer</t>
-  </si>
-  <si>
-    <t>Journal</t>
-  </si>
-  <si>
-    <t>Newsletter</t>
-  </si>
-  <si>
-    <t>Virtualtour</t>
-  </si>
-  <si>
-    <t>Bookbutton</t>
-  </si>
-  <si>
-    <t>Aboutus</t>
-  </si>
-  <si>
-    <t>Feedback</t>
-  </si>
-  <si>
-    <t>TL</t>
-  </si>
-  <si>
-    <t>Türkçe</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Русский</t>
-  </si>
-  <si>
-    <t>Deutsch</t>
-  </si>
-  <si>
-    <t>Español</t>
-  </si>
-  <si>
-    <t>Italiano</t>
-  </si>
-  <si>
-    <t>عربي</t>
-  </si>
-  <si>
-    <t>Weather</t>
   </si>
 </sst>
 </file>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,7 +750,7 @@
     </row>
     <row r="13" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B13" s="14">
         <v>2.4875621890547261</v>
@@ -758,7 +758,7 @@
     </row>
     <row r="14" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="10">
         <v>0</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="15" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="6">
         <v>2.4875621890547261</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="16" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B16" s="6">
         <v>0.49751243781094523</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="18" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B18" s="7">
         <v>2.4875621890547261</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="19" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B19" s="7">
         <v>2.4875621890547261</v>
@@ -806,7 +806,7 @@
     </row>
     <row r="20" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B20" s="7">
         <v>2.4875621890547301</v>
@@ -814,7 +814,7 @@
     </row>
     <row r="21" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B21" s="7">
         <v>1.9900497512437809</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="22" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B22" s="7">
         <v>1.4925373134328357</v>
@@ -830,7 +830,7 @@
     </row>
     <row r="23" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B23" s="7">
         <v>1.4925373134328399</v>
@@ -838,7 +838,7 @@
     </row>
     <row r="24" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B24" s="7">
         <v>1.4925373134328399</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="30" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B30" s="7">
         <v>2.4875621890547261</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="31" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B31" s="7">
         <v>1.9900497512437809</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="32" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="11">
         <v>1.9900497512437809</v>
@@ -910,7 +910,7 @@
     </row>
     <row r="33" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" s="10">
         <v>0</v>
@@ -926,7 +926,7 @@
     </row>
     <row r="35" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B35" s="7">
         <v>2.4875621890547301</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="36" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B36" s="7">
         <v>2.4875621890547261</v>
@@ -942,7 +942,7 @@
     </row>
     <row r="37" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B37" s="10">
         <v>0</v>
@@ -950,7 +950,7 @@
     </row>
     <row r="38" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="7">
         <v>2.4875621890547261</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="39" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B39" s="7">
         <v>2.4875621890547261</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="40" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B40" s="7">
         <v>2.4875621890547261</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="41" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B41" s="7">
         <v>2.4875621890547261</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="42" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B42" s="11">
         <v>2.4875621890547261</v>
@@ -990,7 +990,7 @@
     </row>
     <row r="43" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B43" s="11">
         <v>0</v>
@@ -998,7 +998,7 @@
     </row>
     <row r="44" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B44" s="7">
         <v>0.49751243781094501</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="45" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B45" s="7">
         <v>0.49751243781094501</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="46" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B46" s="11">
         <v>2.4875621890547261</v>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="47" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B47" s="10">
         <v>0</v>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="48" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B48" s="7">
         <v>2.4875621890547261</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="49" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B49" s="7">
         <v>0.49751243781094501</v>
@@ -1046,7 +1046,7 @@
     </row>
     <row r="50" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B50" s="7">
         <v>1.9900497512437809</v>
@@ -1054,7 +1054,7 @@
     </row>
     <row r="51" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B51" s="10">
         <v>0</v>
@@ -1062,7 +1062,7 @@
     </row>
     <row r="52" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B52" s="7">
         <v>2.4875621890547261</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="53" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="B53" s="7">
         <v>2.4875621890547261</v>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="54" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B54" s="7">
         <v>2.4875621890547261</v>
@@ -1086,7 +1086,7 @@
     </row>
     <row r="55" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B55" s="7">
         <v>2.4875621890547261</v>
@@ -1094,7 +1094,7 @@
     </row>
     <row r="56" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B56" s="10">
         <v>0</v>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="57" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B57" s="7">
         <v>1.99004975124378</v>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="58" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B58" s="7">
         <v>1.99004975124378</v>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="59" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B59" s="7">
         <v>1.9900497512437809</v>
@@ -1132,5 +1132,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>